<commit_message>
Guru Bank website linked with TestNG frame work and LoginValid credentials script implemented in project
</commit_message>
<xml_diff>
--- a/SeleniumAutomationProject/src/test/resources/ExcelFiles/TestData.xlsx
+++ b/SeleniumAutomationProject/src/test/resources/ExcelFiles/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="runManager" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t>testname</t>
   </si>
@@ -65,6 +65,20 @@
     <t>For checking</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>loginValidCredentials</t>
+    </r>
+  </si>
+  <si>
+    <t>log in valid credentials</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
@@ -117,6 +131,57 @@
   </si>
   <si>
     <t>Women's Fashion</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mngr525014</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AjebytE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mngr524996</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YnAjemA</t>
+    </r>
+  </si>
+  <si>
+    <t>jayesh</t>
   </si>
 </sst>
 </file>
@@ -738,7 +803,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,6 +811,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
@@ -1073,15 +1141,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.8181818181818" customWidth="1"/>
+    <col min="1" max="1" width="22.3636363636364" customWidth="1"/>
     <col min="2" max="2" width="52.5454545454545" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1112,7 +1180,7 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1129,10 +1197,10 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1146,7 +1214,7 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1161,12 +1229,29 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" ht="22" customHeight="1" spans="1:5">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1179,16 +1264,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.1818181818182" customWidth="1"/>
-    <col min="2" max="4" width="10.3636363636364" customWidth="1"/>
+    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
+    <col min="2" max="3" width="10.3636363636364" customWidth="1"/>
+    <col min="4" max="4" width="12.2727272727273" customWidth="1"/>
     <col min="5" max="5" width="18.0909090909091" customWidth="1"/>
     <col min="6" max="6" width="12.2727272727273" customWidth="1"/>
     <col min="7" max="7" width="24.6363636363636" customWidth="1"/>
@@ -1202,19 +1288,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1225,19 +1311,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1248,19 +1334,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>26</v>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1271,19 +1357,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1294,19 +1380,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>26</v>
+      <c r="F5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1317,19 +1403,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1337,22 +1423,22 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1360,22 +1446,22 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1386,19 +1472,65 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated code with invalid login functionality
</commit_message>
<xml_diff>
--- a/SeleniumAutomationProject/src/test/resources/ExcelFiles/TestData.xlsx
+++ b/SeleniumAutomationProject/src/test/resources/ExcelFiles/TestData.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20401"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPURGE\git\Team_Green\SeleniumAutomationProject\src\test\resources\ExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED00479E-E8FD-4C63-AB87-4022494CB95C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14350" windowHeight="3420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="runManager" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="49">
   <si>
     <t>testname</t>
   </si>
@@ -183,18 +189,36 @@
   <si>
     <t>jayesh</t>
   </si>
+  <si>
+    <t>loginInvalidCredentials</t>
+  </si>
+  <si>
+    <t>log in with Invalid credentials</t>
+  </si>
+  <si>
+    <t>ghowoj</t>
+  </si>
+  <si>
+    <t>49hjfsg</t>
+  </si>
+  <si>
+    <t>slgjlj</t>
+  </si>
+  <si>
+    <t>slgjro</t>
+  </si>
+  <si>
+    <t>ksgnks</t>
+  </si>
+  <si>
+    <t>sgnsf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,346 +232,16 @@
       <name val="Consolas"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -555,255 +249,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -816,68 +268,24 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1135,22 +543,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="52.5454545454545" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="2" max="2" width="52.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1238,7 +646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="22" customHeight="1" spans="1:5">
+    <row r="6" spans="1:5" ht="22" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1246,7 +654,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
@@ -1255,29 +663,44 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.3636363636364" customWidth="1"/>
-    <col min="2" max="3" width="10.3636363636364" customWidth="1"/>
-    <col min="4" max="4" width="12.2727272727273" customWidth="1"/>
-    <col min="5" max="5" width="18.0909090909091" customWidth="1"/>
-    <col min="6" max="6" width="12.2727272727273" customWidth="1"/>
-    <col min="7" max="7" width="24.6363636363636" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="3" width="10.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" customWidth="1"/>
+    <col min="7" max="7" width="24.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1518,7 +941,7 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>38</v>
@@ -1533,8 +956,76 @@
         <v>28</v>
       </c>
     </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Calendar code added and Adds handled dynamically
</commit_message>
<xml_diff>
--- a/SeleniumAutomationProject/src/test/resources/ExcelFiles/TestData.xlsx
+++ b/SeleniumAutomationProject/src/test/resources/ExcelFiles/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6910" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="runManager" sheetId="1" r:id="rId1"/>
@@ -240,7 +240,7 @@
     <t>Female</t>
   </si>
   <si>
-    <t>02/04/2000</t>
+    <t>05052000</t>
   </si>
   <si>
     <t>Marathahalli</t>
@@ -264,12 +264,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -738,16 +739,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -896,7 +897,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6">
@@ -908,7 +909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1390,7 +1391,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>

</xml_diff>